<commit_message>
adicionando uma ideia de Brainstorm
</commit_message>
<xml_diff>
--- a/PastaDesenhosEngenharia/2SIR-ListaRequisitos-SI-Estacionamento.xlsx
+++ b/PastaDesenhosEngenharia/2SIR-ListaRequisitos-SI-Estacionamento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIAP-2024\TEMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rickp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B8BC87-89F4-447E-93D9-595166A4C38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9F3D60-153C-408E-B531-52D629956603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="915" windowWidth="11310" windowHeight="11175" xr2:uid="{B1B7B55A-FA17-40D8-88CB-E329E6023457}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1B7B55A-FA17-40D8-88CB-E329E6023457}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>LISTA DE REQUISITOS - PROJETO SAC (Sistema de atendimento ao consumidor)</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>mudando uma mudança qualquer aqui</t>
   </si>
 </sst>
 </file>
@@ -268,9 +271,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +311,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -414,7 +417,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -556,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -567,7 +570,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,6 +835,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="B19" s="17"/>
       <c r="C19" s="3"/>
       <c r="D19" s="7"/>
@@ -1089,9 +1095,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF4E44C6-AF8F-4DDB-BBAB-2E1C87DCF302}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF4E44C6-AF8F-4DDB-BBAB-2E1C87DCF302}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7bc641a7-997f-4048-a412-d593c6319208"/>
+    <ds:schemaRef ds:uri="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED26A4E4-58F7-4B23-AFC8-2494703F60E1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED26A4E4-58F7-4B23-AFC8-2494703F60E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>